<commit_message>
[DM] UPdated EPRI electricity demand file with state codes, requirements.
</commit_message>
<xml_diff>
--- a/data/electricity-demand/EPRI-US-annual-demand.xlsx
+++ b/data/electricity-demand/EPRI-US-annual-demand.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="82">
   <si>
     <t xml:space="preserve">Source:</t>
   </si>
@@ -154,6 +154,9 @@
     <t xml:space="preserve">State</t>
   </si>
   <si>
+    <t xml:space="preserve">State Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bal Auth</t>
   </si>
   <si>
@@ -163,33 +166,51 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
+    <t xml:space="preserve">VA</t>
+  </si>
+  <si>
     <t xml:space="preserve">PJM</t>
   </si>
   <si>
     <t xml:space="preserve">US-MIDA-PJM</t>
   </si>
   <si>
+    <t xml:space="preserve">TX</t>
+  </si>
+  <si>
     <t xml:space="preserve">ERCOT</t>
   </si>
   <si>
     <t xml:space="preserve">US-TEX-ERCO</t>
   </si>
   <si>
+    <t xml:space="preserve">CA</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAISO</t>
   </si>
   <si>
     <t xml:space="preserve">US-CAL-CISO</t>
   </si>
   <si>
+    <t xml:space="preserve">IL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Also served by MISO</t>
   </si>
   <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
     <t xml:space="preserve">PACW</t>
   </si>
   <si>
     <t xml:space="preserve">US-NW-PACW</t>
   </si>
   <si>
+    <t xml:space="preserve">AZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">SRP</t>
   </si>
   <si>
@@ -199,6 +220,9 @@
     <t xml:space="preserve">Also served by AZPS, PNM, TEPC</t>
   </si>
   <si>
+    <t xml:space="preserve">IA</t>
+  </si>
+  <si>
     <t xml:space="preserve">MISO</t>
   </si>
   <si>
@@ -208,12 +232,18 @@
     <t xml:space="preserve">Also served by SWPP</t>
   </si>
   <si>
+    <t xml:space="preserve">GA</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOCO</t>
   </si>
   <si>
     <t xml:space="preserve">US-SE-SOCO</t>
   </si>
   <si>
+    <t xml:space="preserve">WA</t>
+  </si>
+  <si>
     <t xml:space="preserve">BPA</t>
   </si>
   <si>
@@ -221,6 +251,9 @@
   </si>
   <si>
     <t xml:space="preserve">Also served by PSEI, TPWR, AVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA</t>
   </si>
   <si>
     <t xml:space="preserve">CAGR</t>
@@ -575,7 +608,7 @@
   </sheetPr>
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
@@ -2303,25 +2336,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="17" t="s">
@@ -2329,144 +2362,182 @@
       </c>
       <c r="D1" s="17" t="s">
         <v>45</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>46</v>
+      <c r="B2" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>48</v>
+      <c r="B3" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>50</v>
+      <c r="B4" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>46</v>
+      <c r="B5" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>53</v>
+      <c r="B6" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>55</v>
+      <c r="B7" s="18" t="s">
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>58</v>
+      <c r="B8" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>61</v>
+      <c r="B9" s="18" t="s">
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>63</v>
+      <c r="B10" s="18" t="s">
+        <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>46</v>
+      <c r="B11" s="18" t="s">
+        <v>76</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2487,7 +2558,7 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2509,33 +2580,33 @@
         <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>23</v>
@@ -2553,13 +2624,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>23</v>
@@ -2577,13 +2648,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>20</v>
@@ -2601,13 +2672,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>15</v>
@@ -2625,13 +2696,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>15</v>
@@ -2649,13 +2720,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>15</v>
@@ -2673,13 +2744,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>15</v>
@@ -2697,13 +2768,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>15</v>
@@ -2721,13 +2792,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>15</v>
@@ -2745,13 +2816,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>15</v>
@@ -2772,7 +2843,7 @@
         <v>41</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>18.5291347</v>

</xml_diff>